<commit_message>
Condicionales con "y" "ó" esta en columna k
</commit_message>
<xml_diff>
--- a/Ej. Condicional.xlsx
+++ b/Ej. Condicional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W10\Desktop\Introduccion logica programacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABFDB22C-3939-4650-A27F-D3B9CCDFD875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1DA750-97C5-4354-9FD0-A31E505654DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{817782F4-2F66-49C3-B306-5744E1BED0AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>año</t>
   </si>
@@ -128,6 +128,33 @@
   </si>
   <si>
     <t>mayor o menor</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>panzaso</t>
+  </si>
+  <si>
+    <t>reprobado</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>&gt;0 o &lt;10</t>
+  </si>
+  <si>
+    <t>&gt;=0 y &lt;6</t>
+  </si>
+  <si>
+    <t>&gt;6 y &lt;=10</t>
   </si>
 </sst>
 </file>
@@ -173,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,19 +233,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -278,6 +329,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>55524</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>75286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8827863-F8B3-4914-AED8-A44CD2AED3D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10639425" y="2095500"/>
+          <a:ext cx="13009524" cy="7314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE1EA7A-E6E7-48F7-920C-6C3B937207FE}">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +692,7 @@
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -600,7 +700,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -629,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -664,7 +764,7 @@
         <v>8866</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -699,7 +799,7 @@
         <v>8008</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -734,30 +834,30 @@
         <v>8866</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F8" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -785,11 +885,14 @@
       <c r="I15" t="s">
         <v>26</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -813,19 +916,22 @@
         <v>7</v>
       </c>
       <c r="H16">
-        <f>+AVERAGE(D16:G16)</f>
-        <v>6.5</v>
+        <v>20</v>
       </c>
       <c r="I16" t="str">
         <f>+IF(H16&gt;=6,"Aprobado","Reprobado")</f>
         <v>Aprobado</v>
       </c>
       <c r="J16" t="str">
-        <f>+IF(H16=6,"Panzaso",IF(H16&gt;6,"Aprobado","Reprobado"))</f>
+        <f>+IF(H16=6,"Panzazo",IF(H16&gt;6,"Aprobado","Reprobado"))</f>
         <v>Aprobado</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="str">
+        <f>+IF(AND(H16&gt;6,H16&lt;=10),"Aprobado",IF(H16=6,"Panzazo",IF(AND(H16&lt;6,H16&gt;=0),"Reprobado","error")))</f>
+        <v>error</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -857,11 +963,15 @@
         <v>Aprobado</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17:J20" si="9">+IF(H17=6,"Panzaso",IF(H17&gt;6,"Aprobado","Reprobado"))</f>
+        <f t="shared" ref="J17:J20" si="9">+IF(H17=6,"Panzazo",IF(H17&gt;6,"Aprobado","Reprobado"))</f>
         <v>Aprobado</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="str">
+        <f t="shared" ref="K17:K20" si="10">+IF(AND(H17&gt;6,H17&lt;=10),"Aprobado",IF(H17=6,"Panzazo",IF(AND(H17&lt;6,H17&gt;=0),"Reprobado","error")))</f>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -896,8 +1006,12 @@
         <f t="shared" si="9"/>
         <v>Reprobado</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="10"/>
+        <v>Reprobado</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -932,8 +1046,12 @@
         <f t="shared" si="9"/>
         <v>Aprobado</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="str">
+        <f t="shared" si="10"/>
+        <v>Aprobado</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -966,36 +1084,110 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="9"/>
-        <v>Panzaso</v>
+        <v>Panzazo</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="10"/>
+        <v>Panzazo</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22">
+        <v>6.1</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>5.9</v>
+      </c>
+      <c r="K24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C16:C20">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Mayor de Edad">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Mayor de Edad">
       <formula>NOT(ISERROR(SEARCH("Mayor de Edad",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Menor de Edad">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Menor de Edad">
       <formula>NOT(ISERROR(SEARCH("Menor de Edad",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:I20">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Aprobado">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Aprobado">
       <formula>NOT(ISERROR(SEARCH("Aprobado",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Reprobado">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Reprobado">
       <formula>NOT(ISERROR(SEARCH("Reprobado",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J21">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Reprobado">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Reprobado">
       <formula>NOT(ISERROR(SEARCH("Reprobado",J16)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Aprobado">
+      <formula>NOT(ISERROR(SEARCH("Aprobado",J16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16:K20">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Reprobado">
+      <formula>NOT(ISERROR(SEARCH("Reprobado",K16)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Aprobado">
-      <formula>NOT(ISERROR(SEARCH("Aprobado",J16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Aprobado",K16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>